<commit_message>
search by area and subcat
</commit_message>
<xml_diff>
--- a/Philosophy_j.xlsx
+++ b/Philosophy_j.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Rank</t>
+  </si>
+  <si>
+    <t>SJR</t>
   </si>
   <si>
     <t>Title</t>
@@ -515,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,260 +540,308 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>279</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
+        <v>1.232</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>309</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
+        <v>1.177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <v>68</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
       <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>317</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
+        <v>1.17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>85</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>431</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
+        <v>0.954</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>638</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>833</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
+        <v>0.532</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>851</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
+      <c r="B8">
+        <v>0.521</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
         <v>72</v>
       </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
       <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>945</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
+      <c r="B9">
+        <v>0.464</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>987</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10">
+      <c r="B10">
+        <v>0.44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
       <c r="E10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1244</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
+      <c r="B11">
+        <v>0.298</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
       <c r="E11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1270</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
+      <c r="B12">
+        <v>0.291</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
       <c r="E12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>1343</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
+      <c r="B13">
+        <v>0.261</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
       <c r="E13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>1476</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
+      <c r="B14">
+        <v>0.225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
       <c r="E14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1524</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
+      <c r="B15">
+        <v>0.208</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
       <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>1792</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16">
+      <c r="B16">
+        <v>0.109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>